<commit_message>
Comiteo template carga masiva
</commit_message>
<xml_diff>
--- a/SAREM.Web/Template/Template-Consulta.xlsx
+++ b/SAREM.Web/Template/Template-Consulta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina\Documents\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina\Documents\GitHub\proyecto\SAREM.Web\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,10 +35,10 @@
     <t>ID MEDICO</t>
   </si>
   <si>
-    <t>FECHA INICIO</t>
+    <t>FECHA INICIO - dd/mm/yyyy hh:mm</t>
   </si>
   <si>
-    <t>FECHA FIN</t>
+    <t>FECHA FIN -  dd/mm/yyyy hh:mm</t>
   </si>
 </sst>
 </file>
@@ -87,9 +87,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -371,21 +372,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,6 +402,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Subo los cambios con el turno
Falta modificar los agendar Consulta Paciente, y mover pacientes
consulta lista de espera
</commit_message>
<xml_diff>
--- a/SAREM.Web/Template/Template-Consulta.xlsx
+++ b/SAREM.Web/Template/Template-Consulta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina\Documents\GitHub\proyecto\SAREM.Web\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID LOCAL</t>
   </si>
@@ -39,13 +39,19 @@
   </si>
   <si>
     <t>FECHA FIN -  dd/mm/yyyy hh:mm</t>
+  </si>
+  <si>
+    <t>Cantidad de Pacientes en Consulta</t>
+  </si>
+  <si>
+    <t>Cantidad de Pacientes en Lista de Espera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +62,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,7 +104,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -372,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,6 +398,8 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -402,7 +418,15 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>